<commit_message>
correction to swiss archetypes database for parking
- type_ctrl = T0 was an illegal input, only types T1, T2, T3, T4 exist
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_CH.xlsx
+++ b/cea/databases/archetypes/construction_properties_CH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\CEAforArcGIS\cea\databases\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\CEAforArcGIS\cea\databases\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1139,21 +1139,21 @@
       <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.9296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.53125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.53125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.1328125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.86328125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.1328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="12.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="12" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>70</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="N2" s="12"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="N4" s="12"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>24</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>24</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>24</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>24</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>24</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>25</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>25</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>25</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>25</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>25</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>25</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>25</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>25</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>25</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>25</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>26</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>26</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>26</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>26</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>26</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>26</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>26</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>26</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>26</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>26</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>26</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>26</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>27</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>27</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>27</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>27</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>27</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>27</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>27</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>27</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>27</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>27</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>27</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>27</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>37</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>37</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>37</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>37</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>37</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>37</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>37</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>37</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>37</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>37</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>37</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>37</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>28</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>28</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>28</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>28</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>28</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>28</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>28</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>28</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>28</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>28</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>28</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>28</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>29</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>29</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>29</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>29</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>29</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>29</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>29</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>29</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>29</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>29</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>29</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>29</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>30</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>30</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>30</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>30</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>30</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>30</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>30</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>30</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>30</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>30</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>30</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>30</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>31</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>31</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>31</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>31</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>31</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>31</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>31</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>31</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>31</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>31</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>31</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>31</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>32</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>32</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>32</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>32</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>32</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>32</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>32</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>32</v>
       </c>
@@ -6059,7 +6059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>32</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>32</v>
       </c>
@@ -6135,7 +6135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>32</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
         <v>32</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>33</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>33</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
         <v>33</v>
       </c>
@@ -6325,7 +6325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>33</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>33</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>33</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
         <v>33</v>
       </c>
@@ -6477,7 +6477,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
         <v>33</v>
       </c>
@@ -6515,7 +6515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
         <v>33</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
         <v>33</v>
       </c>
@@ -6591,7 +6591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
         <v>33</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>33</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
         <v>34</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
         <v>34</v>
       </c>
@@ -6743,7 +6743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
         <v>34</v>
       </c>
@@ -6781,7 +6781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>34</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>34</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>34</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>34</v>
       </c>
@@ -6933,7 +6933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>34</v>
       </c>
@@ -6971,7 +6971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>34</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>34</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>34</v>
       </c>
@@ -7085,7 +7085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>34</v>
       </c>
@@ -7123,7 +7123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>35</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>35</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
         <v>35</v>
       </c>
@@ -7237,7 +7237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
         <v>35</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>35</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>35</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>35</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
         <v>35</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
         <v>35</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>35</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
         <v>35</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>35</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>36</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>36</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
         <v>36</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
         <v>36</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
         <v>36</v>
       </c>
@@ -7769,7 +7769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
         <v>36</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="7" t="s">
         <v>36</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
         <v>36</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
         <v>36</v>
       </c>
@@ -7921,7 +7921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
         <v>36</v>
       </c>
@@ -7959,7 +7959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
         <v>36</v>
       </c>
@@ -7997,7 +7997,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
         <v>36</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
         <v>47</v>
       </c>
@@ -8076,7 +8076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
         <v>47</v>
       </c>
@@ -8117,7 +8117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
         <v>47</v>
       </c>
@@ -8158,7 +8158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
         <v>47</v>
       </c>
@@ -8199,7 +8199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
         <v>47</v>
       </c>
@@ -8240,7 +8240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
         <v>47</v>
       </c>
@@ -8281,7 +8281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
         <v>47</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
         <v>47</v>
       </c>
@@ -8363,7 +8363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
         <v>47</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
         <v>47</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
         <v>47</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
         <v>47</v>
       </c>
@@ -8527,7 +8527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="7" t="s">
         <v>48</v>
       </c>
@@ -8567,7 +8567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
         <v>48</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
         <v>48</v>
       </c>
@@ -8647,7 +8647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
         <v>48</v>
       </c>
@@ -8687,7 +8687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
         <v>48</v>
       </c>
@@ -8727,7 +8727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
         <v>48</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
         <v>48</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
         <v>48</v>
       </c>
@@ -8847,7 +8847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
         <v>48</v>
       </c>
@@ -8887,7 +8887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
         <v>48</v>
       </c>
@@ -8927,7 +8927,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204" s="7" t="s">
         <v>48</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
         <v>48</v>
       </c>
@@ -9007,7 +9007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A206" s="7" t="s">
         <v>49</v>
       </c>
@@ -9045,7 +9045,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207" s="7" t="s">
         <v>49</v>
       </c>
@@ -9083,7 +9083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
         <v>49</v>
       </c>
@@ -9121,7 +9121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A209" s="7" t="s">
         <v>49</v>
       </c>
@@ -9159,7 +9159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A210" s="7" t="s">
         <v>49</v>
       </c>
@@ -9197,7 +9197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
         <v>49</v>
       </c>
@@ -9235,7 +9235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
         <v>49</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
         <v>49</v>
       </c>
@@ -9311,7 +9311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
         <v>49</v>
       </c>
@@ -9349,7 +9349,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
         <v>49</v>
       </c>
@@ -9387,7 +9387,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A216" s="7" t="s">
         <v>49</v>
       </c>
@@ -9425,7 +9425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
         <v>49</v>
       </c>
@@ -9477,26 +9477,26 @@
   <dimension ref="A1:I217"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E146" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomRight" activeCell="H158" sqref="H158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.9296875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.19921875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="7.9296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.1328125" style="4"/>
-    <col min="7" max="7" width="9.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.265625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>70</v>
       </c>
@@ -9525,7 +9525,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -9554,7 +9554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -9583,7 +9583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
@@ -9612,7 +9612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -9641,7 +9641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -9670,7 +9670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -9699,7 +9699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -9728,7 +9728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -9757,7 +9757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -9786,7 +9786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -9815,7 +9815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -9873,7 +9873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>24</v>
       </c>
@@ -9931,7 +9931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>24</v>
       </c>
@@ -9960,7 +9960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
@@ -9989,7 +9989,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
@@ -10018,7 +10018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>24</v>
       </c>
@@ -10047,7 +10047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -10076,7 +10076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>24</v>
       </c>
@@ -10105,7 +10105,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
@@ -10134,7 +10134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>24</v>
       </c>
@@ -10163,7 +10163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -10192,7 +10192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>25</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -10279,7 +10279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>25</v>
       </c>
@@ -10308,7 +10308,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>25</v>
       </c>
@@ -10337,7 +10337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>25</v>
       </c>
@@ -10366,7 +10366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -10395,7 +10395,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>25</v>
       </c>
@@ -10424,7 +10424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>25</v>
       </c>
@@ -10453,7 +10453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>25</v>
       </c>
@@ -10482,7 +10482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>25</v>
       </c>
@@ -10511,7 +10511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>25</v>
       </c>
@@ -10540,7 +10540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>25</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>26</v>
       </c>
@@ -10598,7 +10598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>26</v>
       </c>
@@ -10627,7 +10627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>26</v>
       </c>
@@ -10656,7 +10656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>26</v>
       </c>
@@ -10685,7 +10685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>26</v>
       </c>
@@ -10714,7 +10714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>26</v>
       </c>
@@ -10743,7 +10743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>26</v>
       </c>
@@ -10772,7 +10772,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>26</v>
       </c>
@@ -10801,7 +10801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>26</v>
       </c>
@@ -10830,7 +10830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>26</v>
       </c>
@@ -10859,7 +10859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>26</v>
       </c>
@@ -10888,7 +10888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>26</v>
       </c>
@@ -10917,7 +10917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>27</v>
       </c>
@@ -10946,7 +10946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>27</v>
       </c>
@@ -10975,7 +10975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>27</v>
       </c>
@@ -11004,7 +11004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>27</v>
       </c>
@@ -11033,7 +11033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>27</v>
       </c>
@@ -11062,7 +11062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>27</v>
       </c>
@@ -11091,7 +11091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>27</v>
       </c>
@@ -11120,7 +11120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>27</v>
       </c>
@@ -11149,7 +11149,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>27</v>
       </c>
@@ -11178,7 +11178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>27</v>
       </c>
@@ -11207,7 +11207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>27</v>
       </c>
@@ -11236,7 +11236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>27</v>
       </c>
@@ -11265,7 +11265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>37</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>37</v>
       </c>
@@ -11323,7 +11323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>37</v>
       </c>
@@ -11352,7 +11352,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>37</v>
       </c>
@@ -11381,7 +11381,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>37</v>
       </c>
@@ -11410,7 +11410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>37</v>
       </c>
@@ -11439,7 +11439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>37</v>
       </c>
@@ -11468,7 +11468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>37</v>
       </c>
@@ -11497,7 +11497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>37</v>
       </c>
@@ -11526,7 +11526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>37</v>
       </c>
@@ -11555,7 +11555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>37</v>
       </c>
@@ -11584,7 +11584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>37</v>
       </c>
@@ -11613,7 +11613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>28</v>
       </c>
@@ -11642,7 +11642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>28</v>
       </c>
@@ -11671,7 +11671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>28</v>
       </c>
@@ -11700,7 +11700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>28</v>
       </c>
@@ -11729,7 +11729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>28</v>
       </c>
@@ -11758,7 +11758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>28</v>
       </c>
@@ -11787,7 +11787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>28</v>
       </c>
@@ -11816,7 +11816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>28</v>
       </c>
@@ -11845,7 +11845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>28</v>
       </c>
@@ -11874,7 +11874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>28</v>
       </c>
@@ -11903,7 +11903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>28</v>
       </c>
@@ -11932,7 +11932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>28</v>
       </c>
@@ -11961,7 +11961,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>29</v>
       </c>
@@ -11990,7 +11990,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>29</v>
       </c>
@@ -12019,7 +12019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>29</v>
       </c>
@@ -12048,7 +12048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>29</v>
       </c>
@@ -12077,7 +12077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>29</v>
       </c>
@@ -12106,7 +12106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>29</v>
       </c>
@@ -12135,7 +12135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>29</v>
       </c>
@@ -12164,7 +12164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>29</v>
       </c>
@@ -12193,7 +12193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>29</v>
       </c>
@@ -12222,7 +12222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>29</v>
       </c>
@@ -12251,7 +12251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>29</v>
       </c>
@@ -12280,7 +12280,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>29</v>
       </c>
@@ -12309,7 +12309,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>30</v>
       </c>
@@ -12338,7 +12338,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>30</v>
       </c>
@@ -12367,7 +12367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>30</v>
       </c>
@@ -12396,7 +12396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>30</v>
       </c>
@@ -12425,7 +12425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>30</v>
       </c>
@@ -12454,7 +12454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>30</v>
       </c>
@@ -12483,7 +12483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>30</v>
       </c>
@@ -12512,7 +12512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>30</v>
       </c>
@@ -12541,7 +12541,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>30</v>
       </c>
@@ -12570,7 +12570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>30</v>
       </c>
@@ -12599,7 +12599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>30</v>
       </c>
@@ -12628,7 +12628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>30</v>
       </c>
@@ -12657,7 +12657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>31</v>
       </c>
@@ -12686,7 +12686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>31</v>
       </c>
@@ -12715,7 +12715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>31</v>
       </c>
@@ -12744,7 +12744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>31</v>
       </c>
@@ -12773,7 +12773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>31</v>
       </c>
@@ -12802,7 +12802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>31</v>
       </c>
@@ -12831,7 +12831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>31</v>
       </c>
@@ -12860,7 +12860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>31</v>
       </c>
@@ -12889,7 +12889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>31</v>
       </c>
@@ -12918,7 +12918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>31</v>
       </c>
@@ -12947,7 +12947,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>31</v>
       </c>
@@ -12976,7 +12976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>31</v>
       </c>
@@ -13005,7 +13005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>32</v>
       </c>
@@ -13034,7 +13034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>32</v>
       </c>
@@ -13063,7 +13063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>32</v>
       </c>
@@ -13092,7 +13092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>32</v>
       </c>
@@ -13121,7 +13121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>32</v>
       </c>
@@ -13150,7 +13150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>32</v>
       </c>
@@ -13179,7 +13179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>32</v>
       </c>
@@ -13208,7 +13208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>32</v>
       </c>
@@ -13237,7 +13237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>32</v>
       </c>
@@ -13266,7 +13266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>32</v>
       </c>
@@ -13295,7 +13295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>32</v>
       </c>
@@ -13324,7 +13324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
         <v>32</v>
       </c>
@@ -13353,7 +13353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>33</v>
       </c>
@@ -13382,7 +13382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>33</v>
       </c>
@@ -13411,7 +13411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
         <v>33</v>
       </c>
@@ -13440,7 +13440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>33</v>
       </c>
@@ -13469,7 +13469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>33</v>
       </c>
@@ -13498,7 +13498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>33</v>
       </c>
@@ -13527,7 +13527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
         <v>33</v>
       </c>
@@ -13556,7 +13556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
         <v>33</v>
       </c>
@@ -13585,7 +13585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
         <v>33</v>
       </c>
@@ -13614,7 +13614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
         <v>33</v>
       </c>
@@ -13643,7 +13643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
         <v>33</v>
       </c>
@@ -13672,7 +13672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>33</v>
       </c>
@@ -13701,7 +13701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
         <v>34</v>
       </c>
@@ -13730,7 +13730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
         <v>34</v>
       </c>
@@ -13759,7 +13759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
         <v>34</v>
       </c>
@@ -13788,7 +13788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>34</v>
       </c>
@@ -13817,7 +13817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>34</v>
       </c>
@@ -13846,7 +13846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>34</v>
       </c>
@@ -13875,7 +13875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>34</v>
       </c>
@@ -13904,7 +13904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>34</v>
       </c>
@@ -13933,7 +13933,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>34</v>
       </c>
@@ -13962,7 +13962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>34</v>
       </c>
@@ -13991,7 +13991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>34</v>
       </c>
@@ -14020,7 +14020,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>34</v>
       </c>
@@ -14049,7 +14049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>35</v>
       </c>
@@ -14072,13 +14072,13 @@
         <v>10</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I158" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>35</v>
       </c>
@@ -14101,13 +14101,13 @@
         <v>10</v>
       </c>
       <c r="H159" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I159" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
         <v>35</v>
       </c>
@@ -14130,13 +14130,13 @@
         <v>10</v>
       </c>
       <c r="H160" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I160" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
         <v>35</v>
       </c>
@@ -14159,13 +14159,13 @@
         <v>10</v>
       </c>
       <c r="H161" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I161" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>35</v>
       </c>
@@ -14188,13 +14188,13 @@
         <v>10</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I162" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>35</v>
       </c>
@@ -14217,13 +14217,13 @@
         <v>10</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I163" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>35</v>
       </c>
@@ -14246,13 +14246,13 @@
         <v>10</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I164" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
         <v>35</v>
       </c>
@@ -14275,13 +14275,13 @@
         <v>10</v>
       </c>
       <c r="H165" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I165" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
         <v>35</v>
       </c>
@@ -14304,13 +14304,13 @@
         <v>10</v>
       </c>
       <c r="H166" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I166" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>35</v>
       </c>
@@ -14333,13 +14333,13 @@
         <v>10</v>
       </c>
       <c r="H167" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I167" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
         <v>35</v>
       </c>
@@ -14362,13 +14362,13 @@
         <v>10</v>
       </c>
       <c r="H168" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I168" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>35</v>
       </c>
@@ -14391,13 +14391,13 @@
         <v>10</v>
       </c>
       <c r="H169" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I169" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>36</v>
       </c>
@@ -14426,7 +14426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>36</v>
       </c>
@@ -14455,7 +14455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
         <v>36</v>
       </c>
@@ -14484,7 +14484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
         <v>36</v>
       </c>
@@ -14513,7 +14513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
         <v>36</v>
       </c>
@@ -14542,7 +14542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
         <v>36</v>
       </c>
@@ -14571,7 +14571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="7" t="s">
         <v>36</v>
       </c>
@@ -14600,7 +14600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
         <v>36</v>
       </c>
@@ -14629,7 +14629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
         <v>36</v>
       </c>
@@ -14658,7 +14658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
         <v>36</v>
       </c>
@@ -14687,7 +14687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
         <v>36</v>
       </c>
@@ -14716,7 +14716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
         <v>36</v>
       </c>
@@ -14745,7 +14745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
         <v>47</v>
       </c>
@@ -14779,7 +14779,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
         <v>47</v>
       </c>
@@ -14813,7 +14813,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
         <v>47</v>
       </c>
@@ -14847,7 +14847,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
         <v>47</v>
       </c>
@@ -14881,7 +14881,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
         <v>47</v>
       </c>
@@ -14915,7 +14915,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
         <v>47</v>
       </c>
@@ -14949,7 +14949,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
         <v>47</v>
       </c>
@@ -14983,7 +14983,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
         <v>47</v>
       </c>
@@ -15017,7 +15017,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
         <v>47</v>
       </c>
@@ -15051,7 +15051,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
         <v>47</v>
       </c>
@@ -15085,7 +15085,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
         <v>47</v>
       </c>
@@ -15119,7 +15119,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
         <v>47</v>
       </c>
@@ -15153,7 +15153,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="7" t="s">
         <v>48</v>
       </c>
@@ -15184,7 +15184,7 @@
         <v>T0</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
         <v>48</v>
       </c>
@@ -15215,7 +15215,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
         <v>48</v>
       </c>
@@ -15246,7 +15246,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
         <v>48</v>
       </c>
@@ -15277,7 +15277,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
         <v>48</v>
       </c>
@@ -15308,7 +15308,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
         <v>48</v>
       </c>
@@ -15339,7 +15339,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
         <v>48</v>
       </c>
@@ -15370,7 +15370,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
         <v>48</v>
       </c>
@@ -15401,7 +15401,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
         <v>48</v>
       </c>
@@ -15432,7 +15432,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
         <v>48</v>
       </c>
@@ -15463,7 +15463,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="7" t="s">
         <v>48</v>
       </c>
@@ -15494,7 +15494,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
         <v>48</v>
       </c>
@@ -15525,7 +15525,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="7" t="s">
         <v>49</v>
       </c>
@@ -15554,7 +15554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="7" t="s">
         <v>49</v>
       </c>
@@ -15583,7 +15583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
         <v>49</v>
       </c>
@@ -15612,7 +15612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="7" t="s">
         <v>49</v>
       </c>
@@ -15641,7 +15641,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="7" t="s">
         <v>49</v>
       </c>
@@ -15670,7 +15670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
         <v>49</v>
       </c>
@@ -15699,7 +15699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
         <v>49</v>
       </c>
@@ -15728,7 +15728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
         <v>49</v>
       </c>
@@ -15757,7 +15757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
         <v>49</v>
       </c>
@@ -15786,7 +15786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
         <v>49</v>
       </c>
@@ -15815,7 +15815,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="7" t="s">
         <v>49</v>
       </c>
@@ -15844,7 +15844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
         <v>49</v>
       </c>
@@ -15887,18 +15887,18 @@
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.86328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.73046875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1328125" style="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -15918,7 +15918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -15938,7 +15938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -15958,7 +15958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>25</v>
       </c>
@@ -15978,7 +15978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
@@ -15998,7 +15998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -16018,7 +16018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
@@ -16038,7 +16038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
@@ -16059,7 +16059,7 @@
         <v>25.15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -16079,7 +16079,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>30</v>
       </c>
@@ -16099,7 +16099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -16119,7 +16119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -16139,7 +16139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
@@ -16159,7 +16159,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
@@ -16179,7 +16179,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
@@ -16199,7 +16199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -16219,7 +16219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -16240,7 +16240,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>48</v>
       </c>
@@ -16260,7 +16260,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>49</v>
       </c>
@@ -16294,21 +16294,21 @@
       <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.73046875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -16340,7 +16340,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -16372,7 +16372,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -16406,7 +16406,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>25</v>
       </c>
@@ -16438,7 +16438,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>26</v>
       </c>
@@ -16470,7 +16470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -16504,7 +16504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
@@ -16536,7 +16536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
@@ -16568,7 +16568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -16600,7 +16600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>30</v>
       </c>
@@ -16632,7 +16632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -16664,7 +16664,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -16696,7 +16696,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
@@ -16728,7 +16728,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
@@ -16760,7 +16760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
@@ -16792,7 +16792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -16824,7 +16824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -16861,7 +16861,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>48</v>
       </c>
@@ -16895,7 +16895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>49</v>
       </c>
@@ -16927,7 +16927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G22" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting `Hs` values in archetypes
These were inconsistently defined for MULTI_RES and SERVERROOM buildings
renovated after 2006.
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_CH.xlsx
+++ b/cea/databases/archetypes/construction_properties_CH.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\CEAforArcGIS\cea\databases\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/C/Users/User/Documents/GitHub/CEAforArcGIS/cea/databases/archetypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16140" tabRatio="785" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="INDOOR_COMFORT" sheetId="6" r:id="rId3"/>
     <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1132,28 +1132,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N217"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E214" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="E235" sqref="E235"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="12.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>70</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="N2" s="12"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="N4" s="12"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>24</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>24</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>24</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>24</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>24</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>68</v>
       </c>
       <c r="E24" s="3">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="F24" s="3">
         <v>0.2</v>
@@ -2069,7 +2069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>68</v>
       </c>
       <c r="E25" s="3">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="F25" s="3">
         <v>0.2</v>
@@ -2107,7 +2107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>25</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>25</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>25</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>25</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>25</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>25</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>25</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>25</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>25</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>25</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>26</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>26</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>26</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>26</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>26</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>26</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>26</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>26</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>26</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>26</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>26</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>26</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>27</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>27</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>27</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>27</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>27</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>27</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>27</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>27</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>27</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>27</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>27</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>27</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>37</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>37</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>37</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>37</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>37</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>37</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>37</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>37</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
         <v>37</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>37</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>37</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
         <v>37</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
         <v>28</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
         <v>28</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
         <v>28</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>28</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
         <v>28</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>28</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
         <v>28</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
         <v>28</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
         <v>28</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
         <v>28</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>28</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
         <v>28</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>29</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>29</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>29</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>29</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
         <v>29</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>29</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>29</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>29</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>29</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>29</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>29</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
         <v>29</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
         <v>30</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
         <v>30</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
         <v>30</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
         <v>30</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
         <v>30</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
         <v>30</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
         <v>30</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
         <v>30</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
         <v>30</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
         <v>30</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
         <v>30</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
         <v>30</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
         <v>31</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
         <v>31</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
         <v>31</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
         <v>31</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
         <v>31</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
         <v>31</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
         <v>31</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
         <v>31</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
         <v>31</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
         <v>31</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
         <v>31</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
         <v>31</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
         <v>32</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
         <v>32</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
         <v>32</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
         <v>32</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
         <v>32</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
         <v>32</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
         <v>32</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="s">
         <v>32</v>
       </c>
@@ -6059,7 +6059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
         <v>32</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
         <v>32</v>
       </c>
@@ -6135,7 +6135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
         <v>32</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
         <v>32</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
         <v>33</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
         <v>33</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
         <v>33</v>
       </c>
@@ -6325,7 +6325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
         <v>33</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
         <v>33</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
         <v>33</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
         <v>33</v>
       </c>
@@ -6477,7 +6477,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
         <v>33</v>
       </c>
@@ -6515,7 +6515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
         <v>33</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
         <v>33</v>
       </c>
@@ -6591,7 +6591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
         <v>33</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
         <v>33</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" s="7" t="s">
         <v>34</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="s">
         <v>34</v>
       </c>
@@ -6743,7 +6743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" s="7" t="s">
         <v>34</v>
       </c>
@@ -6781,7 +6781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" s="7" t="s">
         <v>34</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" s="7" t="s">
         <v>34</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
         <v>34</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" s="7" t="s">
         <v>34</v>
       </c>
@@ -6933,7 +6933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
         <v>34</v>
       </c>
@@ -6971,7 +6971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
         <v>34</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
         <v>34</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
         <v>34</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>68</v>
       </c>
       <c r="E156" s="3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F156" s="3">
         <v>0.1</v>
@@ -7085,7 +7085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="s">
         <v>34</v>
       </c>
@@ -7099,7 +7099,7 @@
         <v>68</v>
       </c>
       <c r="E157" s="3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F157" s="3">
         <v>0.1</v>
@@ -7123,7 +7123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" s="7" t="s">
         <v>35</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" s="7" t="s">
         <v>35</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" s="7" t="s">
         <v>35</v>
       </c>
@@ -7237,7 +7237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" s="7" t="s">
         <v>35</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" s="7" t="s">
         <v>35</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
         <v>35</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
         <v>35</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="s">
         <v>35</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
         <v>35</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="s">
         <v>35</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A168" s="7" t="s">
         <v>35</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A169" s="7" t="s">
         <v>35</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170" s="7" t="s">
         <v>36</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A171" s="7" t="s">
         <v>36</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172" s="7" t="s">
         <v>36</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="s">
         <v>36</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
         <v>36</v>
       </c>
@@ -7769,7 +7769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="s">
         <v>36</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A176" s="7" t="s">
         <v>36</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="s">
         <v>36</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178" s="7" t="s">
         <v>36</v>
       </c>
@@ -7921,7 +7921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179" s="7" t="s">
         <v>36</v>
       </c>
@@ -7959,7 +7959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180" s="7" t="s">
         <v>36</v>
       </c>
@@ -7997,7 +7997,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181" s="7" t="s">
         <v>36</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" s="7" t="s">
         <v>47</v>
       </c>
@@ -8076,7 +8076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
         <v>47</v>
       </c>
@@ -8117,7 +8117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
         <v>47</v>
       </c>
@@ -8158,7 +8158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A185" s="7" t="s">
         <v>47</v>
       </c>
@@ -8199,7 +8199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
         <v>47</v>
       </c>
@@ -8240,7 +8240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
         <v>47</v>
       </c>
@@ -8281,7 +8281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
         <v>47</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
         <v>47</v>
       </c>
@@ -8363,7 +8363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
         <v>47</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="s">
         <v>47</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
         <v>47</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="s">
         <v>47</v>
       </c>
@@ -8527,7 +8527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194" s="7" t="s">
         <v>48</v>
       </c>
@@ -8567,7 +8567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195" s="7" t="s">
         <v>48</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A196" s="7" t="s">
         <v>48</v>
       </c>
@@ -8647,7 +8647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A197" s="7" t="s">
         <v>48</v>
       </c>
@@ -8687,7 +8687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A198" s="7" t="s">
         <v>48</v>
       </c>
@@ -8727,7 +8727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199" s="7" t="s">
         <v>48</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A200" s="7" t="s">
         <v>48</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201" s="7" t="s">
         <v>48</v>
       </c>
@@ -8847,7 +8847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A202" s="7" t="s">
         <v>48</v>
       </c>
@@ -8887,7 +8887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A203" s="7" t="s">
         <v>48</v>
       </c>
@@ -8927,7 +8927,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A204" s="7" t="s">
         <v>48</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A205" s="7" t="s">
         <v>48</v>
       </c>
@@ -9007,7 +9007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206" s="7" t="s">
         <v>49</v>
       </c>
@@ -9045,7 +9045,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207" s="7" t="s">
         <v>49</v>
       </c>
@@ -9083,7 +9083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208" s="7" t="s">
         <v>49</v>
       </c>
@@ -9121,7 +9121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A209" s="7" t="s">
         <v>49</v>
       </c>
@@ -9159,7 +9159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A210" s="7" t="s">
         <v>49</v>
       </c>
@@ -9197,7 +9197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A211" s="7" t="s">
         <v>49</v>
       </c>
@@ -9235,7 +9235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A212" s="7" t="s">
         <v>49</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A213" s="7" t="s">
         <v>49</v>
       </c>
@@ -9311,7 +9311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A214" s="7" t="s">
         <v>49</v>
       </c>
@@ -9349,7 +9349,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A215" s="7" t="s">
         <v>49</v>
       </c>
@@ -9387,7 +9387,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A216" s="7" t="s">
         <v>49</v>
       </c>
@@ -9425,7 +9425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A217" s="7" t="s">
         <v>49</v>
       </c>
@@ -9476,27 +9476,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E146" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E144" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="H158" sqref="H158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="14" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>70</v>
       </c>
@@ -9525,7 +9525,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -9554,7 +9554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -9583,7 +9583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
@@ -9612,7 +9612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -9641,7 +9641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -9670,7 +9670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -9699,7 +9699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -9728,7 +9728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -9757,7 +9757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -9786,7 +9786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -9815,7 +9815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -9873,7 +9873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>24</v>
       </c>
@@ -9931,7 +9931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>24</v>
       </c>
@@ -9960,7 +9960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
@@ -9989,7 +9989,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
@@ -10018,7 +10018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>24</v>
       </c>
@@ -10047,7 +10047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -10076,7 +10076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>24</v>
       </c>
@@ -10105,7 +10105,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
@@ -10134,7 +10134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>24</v>
       </c>
@@ -10163,7 +10163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -10192,7 +10192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>25</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -10279,7 +10279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>25</v>
       </c>
@@ -10308,7 +10308,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>25</v>
       </c>
@@ -10337,7 +10337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>25</v>
       </c>
@@ -10366,7 +10366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -10395,7 +10395,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>25</v>
       </c>
@@ -10424,7 +10424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>25</v>
       </c>
@@ -10453,7 +10453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>25</v>
       </c>
@@ -10482,7 +10482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>25</v>
       </c>
@@ -10511,7 +10511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>25</v>
       </c>
@@ -10540,7 +10540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>25</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>26</v>
       </c>
@@ -10598,7 +10598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>26</v>
       </c>
@@ -10627,7 +10627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>26</v>
       </c>
@@ -10656,7 +10656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>26</v>
       </c>
@@ -10685,7 +10685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>26</v>
       </c>
@@ -10714,7 +10714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>26</v>
       </c>
@@ -10743,7 +10743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>26</v>
       </c>
@@ -10772,7 +10772,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>26</v>
       </c>
@@ -10801,7 +10801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>26</v>
       </c>
@@ -10830,7 +10830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>26</v>
       </c>
@@ -10859,7 +10859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>26</v>
       </c>
@@ -10888,7 +10888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>26</v>
       </c>
@@ -10917,7 +10917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>27</v>
       </c>
@@ -10946,7 +10946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>27</v>
       </c>
@@ -10975,7 +10975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>27</v>
       </c>
@@ -11004,7 +11004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>27</v>
       </c>
@@ -11033,7 +11033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>27</v>
       </c>
@@ -11062,7 +11062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>27</v>
       </c>
@@ -11091,7 +11091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>27</v>
       </c>
@@ -11120,7 +11120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>27</v>
       </c>
@@ -11149,7 +11149,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>27</v>
       </c>
@@ -11178,7 +11178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>27</v>
       </c>
@@ -11207,7 +11207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>27</v>
       </c>
@@ -11236,7 +11236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>27</v>
       </c>
@@ -11265,7 +11265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>37</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>37</v>
       </c>
@@ -11323,7 +11323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>37</v>
       </c>
@@ -11352,7 +11352,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>37</v>
       </c>
@@ -11381,7 +11381,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>37</v>
       </c>
@@ -11410,7 +11410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>37</v>
       </c>
@@ -11439,7 +11439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>37</v>
       </c>
@@ -11468,7 +11468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>37</v>
       </c>
@@ -11497,7 +11497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
         <v>37</v>
       </c>
@@ -11526,7 +11526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>37</v>
       </c>
@@ -11555,7 +11555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>37</v>
       </c>
@@ -11584,7 +11584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
         <v>37</v>
       </c>
@@ -11613,7 +11613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
         <v>28</v>
       </c>
@@ -11642,7 +11642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
         <v>28</v>
       </c>
@@ -11671,7 +11671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
         <v>28</v>
       </c>
@@ -11700,7 +11700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>28</v>
       </c>
@@ -11729,7 +11729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
         <v>28</v>
       </c>
@@ -11758,7 +11758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>28</v>
       </c>
@@ -11787,7 +11787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
         <v>28</v>
       </c>
@@ -11816,7 +11816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
         <v>28</v>
       </c>
@@ -11845,7 +11845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
         <v>28</v>
       </c>
@@ -11874,7 +11874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
         <v>28</v>
       </c>
@@ -11903,7 +11903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>28</v>
       </c>
@@ -11932,7 +11932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
         <v>28</v>
       </c>
@@ -11961,7 +11961,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>29</v>
       </c>
@@ -11990,7 +11990,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>29</v>
       </c>
@@ -12019,7 +12019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>29</v>
       </c>
@@ -12048,7 +12048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>29</v>
       </c>
@@ -12077,7 +12077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
         <v>29</v>
       </c>
@@ -12106,7 +12106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>29</v>
       </c>
@@ -12135,7 +12135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>29</v>
       </c>
@@ -12164,7 +12164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>29</v>
       </c>
@@ -12193,7 +12193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>29</v>
       </c>
@@ -12222,7 +12222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>29</v>
       </c>
@@ -12251,7 +12251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>29</v>
       </c>
@@ -12280,7 +12280,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
         <v>29</v>
       </c>
@@ -12309,7 +12309,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
         <v>30</v>
       </c>
@@ -12338,7 +12338,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
         <v>30</v>
       </c>
@@ -12367,7 +12367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
         <v>30</v>
       </c>
@@ -12396,7 +12396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
         <v>30</v>
       </c>
@@ -12425,7 +12425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
         <v>30</v>
       </c>
@@ -12454,7 +12454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
         <v>30</v>
       </c>
@@ -12483,7 +12483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
         <v>30</v>
       </c>
@@ -12512,7 +12512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
         <v>30</v>
       </c>
@@ -12541,7 +12541,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
         <v>30</v>
       </c>
@@ -12570,7 +12570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
         <v>30</v>
       </c>
@@ -12599,7 +12599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
         <v>30</v>
       </c>
@@ -12628,7 +12628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
         <v>30</v>
       </c>
@@ -12657,7 +12657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
         <v>31</v>
       </c>
@@ -12686,7 +12686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
         <v>31</v>
       </c>
@@ -12715,7 +12715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
         <v>31</v>
       </c>
@@ -12744,7 +12744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
         <v>31</v>
       </c>
@@ -12773,7 +12773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
         <v>31</v>
       </c>
@@ -12802,7 +12802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
         <v>31</v>
       </c>
@@ -12831,7 +12831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
         <v>31</v>
       </c>
@@ -12860,7 +12860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
         <v>31</v>
       </c>
@@ -12889,7 +12889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
         <v>31</v>
       </c>
@@ -12918,7 +12918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
         <v>31</v>
       </c>
@@ -12947,7 +12947,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
         <v>31</v>
       </c>
@@ -12976,7 +12976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
         <v>31</v>
       </c>
@@ -13005,7 +13005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
         <v>32</v>
       </c>
@@ -13034,7 +13034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
         <v>32</v>
       </c>
@@ -13063,7 +13063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
         <v>32</v>
       </c>
@@ -13092,7 +13092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
         <v>32</v>
       </c>
@@ -13121,7 +13121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
         <v>32</v>
       </c>
@@ -13150,7 +13150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
         <v>32</v>
       </c>
@@ -13179,7 +13179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
         <v>32</v>
       </c>
@@ -13208,7 +13208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="s">
         <v>32</v>
       </c>
@@ -13237,7 +13237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
         <v>32</v>
       </c>
@@ -13266,7 +13266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
         <v>32</v>
       </c>
@@ -13295,7 +13295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
         <v>32</v>
       </c>
@@ -13324,7 +13324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
         <v>32</v>
       </c>
@@ -13353,7 +13353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
         <v>33</v>
       </c>
@@ -13382,7 +13382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
         <v>33</v>
       </c>
@@ -13411,7 +13411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
         <v>33</v>
       </c>
@@ -13440,7 +13440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
         <v>33</v>
       </c>
@@ -13469,7 +13469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
         <v>33</v>
       </c>
@@ -13498,7 +13498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
         <v>33</v>
       </c>
@@ -13527,7 +13527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
         <v>33</v>
       </c>
@@ -13556,7 +13556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
         <v>33</v>
       </c>
@@ -13585,7 +13585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
         <v>33</v>
       </c>
@@ -13614,7 +13614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
         <v>33</v>
       </c>
@@ -13643,7 +13643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
         <v>33</v>
       </c>
@@ -13672,7 +13672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
         <v>33</v>
       </c>
@@ -13701,7 +13701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="7" t="s">
         <v>34</v>
       </c>
@@ -13730,7 +13730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="s">
         <v>34</v>
       </c>
@@ -13759,7 +13759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="7" t="s">
         <v>34</v>
       </c>
@@ -13788,7 +13788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="7" t="s">
         <v>34</v>
       </c>
@@ -13817,7 +13817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="7" t="s">
         <v>34</v>
       </c>
@@ -13846,7 +13846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
         <v>34</v>
       </c>
@@ -13875,7 +13875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="7" t="s">
         <v>34</v>
       </c>
@@ -13904,7 +13904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
         <v>34</v>
       </c>
@@ -13933,7 +13933,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
         <v>34</v>
       </c>
@@ -13962,7 +13962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
         <v>34</v>
       </c>
@@ -13991,7 +13991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
         <v>34</v>
       </c>
@@ -14020,7 +14020,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="s">
         <v>34</v>
       </c>
@@ -14049,7 +14049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="7" t="s">
         <v>35</v>
       </c>
@@ -14078,7 +14078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="7" t="s">
         <v>35</v>
       </c>
@@ -14107,7 +14107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="7" t="s">
         <v>35</v>
       </c>
@@ -14136,7 +14136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="7" t="s">
         <v>35</v>
       </c>
@@ -14165,7 +14165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="7" t="s">
         <v>35</v>
       </c>
@@ -14194,7 +14194,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
         <v>35</v>
       </c>
@@ -14223,7 +14223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
         <v>35</v>
       </c>
@@ -14252,7 +14252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="s">
         <v>35</v>
       </c>
@@ -14281,7 +14281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
         <v>35</v>
       </c>
@@ -14310,7 +14310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="s">
         <v>35</v>
       </c>
@@ -14339,7 +14339,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="7" t="s">
         <v>35</v>
       </c>
@@ -14368,7 +14368,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="7" t="s">
         <v>35</v>
       </c>
@@ -14397,7 +14397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="7" t="s">
         <v>36</v>
       </c>
@@ -14426,7 +14426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" s="7" t="s">
         <v>36</v>
       </c>
@@ -14455,7 +14455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="7" t="s">
         <v>36</v>
       </c>
@@ -14484,7 +14484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="s">
         <v>36</v>
       </c>
@@ -14513,7 +14513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
         <v>36</v>
       </c>
@@ -14542,7 +14542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="s">
         <v>36</v>
       </c>
@@ -14571,7 +14571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="7" t="s">
         <v>36</v>
       </c>
@@ -14600,7 +14600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="s">
         <v>36</v>
       </c>
@@ -14629,7 +14629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="7" t="s">
         <v>36</v>
       </c>
@@ -14658,7 +14658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="7" t="s">
         <v>36</v>
       </c>
@@ -14687,7 +14687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="7" t="s">
         <v>36</v>
       </c>
@@ -14716,7 +14716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="7" t="s">
         <v>36</v>
       </c>
@@ -14745,7 +14745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="7" t="s">
         <v>47</v>
       </c>
@@ -14779,7 +14779,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
         <v>47</v>
       </c>
@@ -14813,7 +14813,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
         <v>47</v>
       </c>
@@ -14847,7 +14847,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" s="7" t="s">
         <v>47</v>
       </c>
@@ -14881,7 +14881,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
         <v>47</v>
       </c>
@@ -14915,7 +14915,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
         <v>47</v>
       </c>
@@ -14949,7 +14949,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
         <v>47</v>
       </c>
@@ -14983,7 +14983,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
         <v>47</v>
       </c>
@@ -15017,7 +15017,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
         <v>47</v>
       </c>
@@ -15051,7 +15051,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="s">
         <v>47</v>
       </c>
@@ -15085,7 +15085,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
         <v>47</v>
       </c>
@@ -15119,7 +15119,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="s">
         <v>47</v>
       </c>
@@ -15153,7 +15153,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" s="7" t="s">
         <v>48</v>
       </c>
@@ -15184,7 +15184,7 @@
         <v>T0</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" s="7" t="s">
         <v>48</v>
       </c>
@@ -15215,7 +15215,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" s="7" t="s">
         <v>48</v>
       </c>
@@ -15246,7 +15246,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" s="7" t="s">
         <v>48</v>
       </c>
@@ -15277,7 +15277,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A198" s="7" t="s">
         <v>48</v>
       </c>
@@ -15308,7 +15308,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A199" s="7" t="s">
         <v>48</v>
       </c>
@@ -15339,7 +15339,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A200" s="7" t="s">
         <v>48</v>
       </c>
@@ -15370,7 +15370,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A201" s="7" t="s">
         <v>48</v>
       </c>
@@ -15401,7 +15401,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A202" s="7" t="s">
         <v>48</v>
       </c>
@@ -15432,7 +15432,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A203" s="7" t="s">
         <v>48</v>
       </c>
@@ -15463,7 +15463,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A204" s="7" t="s">
         <v>48</v>
       </c>
@@ -15494,7 +15494,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A205" s="7" t="s">
         <v>48</v>
       </c>
@@ -15525,7 +15525,7 @@
         <v>T1</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A206" s="7" t="s">
         <v>49</v>
       </c>
@@ -15554,7 +15554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A207" s="7" t="s">
         <v>49</v>
       </c>
@@ -15583,7 +15583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A208" s="7" t="s">
         <v>49</v>
       </c>
@@ -15612,7 +15612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A209" s="7" t="s">
         <v>49</v>
       </c>
@@ -15641,7 +15641,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A210" s="7" t="s">
         <v>49</v>
       </c>
@@ -15670,7 +15670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A211" s="7" t="s">
         <v>49</v>
       </c>
@@ -15699,7 +15699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A212" s="7" t="s">
         <v>49</v>
       </c>
@@ -15728,7 +15728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A213" s="7" t="s">
         <v>49</v>
       </c>
@@ -15757,7 +15757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A214" s="7" t="s">
         <v>49</v>
       </c>
@@ -15786,7 +15786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A215" s="7" t="s">
         <v>49</v>
       </c>
@@ -15815,7 +15815,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A216" s="7" t="s">
         <v>49</v>
       </c>
@@ -15844,7 +15844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A217" s="7" t="s">
         <v>49</v>
       </c>
@@ -15887,18 +15887,18 @@
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -15918,7 +15918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -15938,7 +15938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -15958,7 +15958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>25</v>
       </c>
@@ -15978,7 +15978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
@@ -15998,7 +15998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -16018,7 +16018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
@@ -16038,7 +16038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
@@ -16059,7 +16059,7 @@
         <v>25.15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -16079,7 +16079,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>30</v>
       </c>
@@ -16099,7 +16099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -16119,7 +16119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -16139,7 +16139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
@@ -16159,7 +16159,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
@@ -16179,7 +16179,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
@@ -16199,7 +16199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -16219,7 +16219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -16240,7 +16240,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>48</v>
       </c>
@@ -16260,7 +16260,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>49</v>
       </c>
@@ -16294,21 +16294,21 @@
       <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -16340,7 +16340,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -16372,7 +16372,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -16406,7 +16406,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>25</v>
       </c>
@@ -16438,7 +16438,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>26</v>
       </c>
@@ -16470,7 +16470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -16504,7 +16504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
@@ -16536,7 +16536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
@@ -16568,7 +16568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -16600,7 +16600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>30</v>
       </c>
@@ -16632,7 +16632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -16664,7 +16664,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -16696,7 +16696,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
@@ -16728,7 +16728,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
@@ -16760,7 +16760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
@@ -16792,7 +16792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -16824,7 +16824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -16861,7 +16861,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>48</v>
       </c>
@@ -16895,7 +16895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>49</v>
       </c>
@@ -16927,7 +16927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G22" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating reference values for archetypes
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_CH.xlsx
+++ b/cea/databases/archetypes/construction_properties_CH.xlsx
@@ -16297,7 +16297,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16654,12 +16654,10 @@
         <v>20</v>
       </c>
       <c r="K9" s="6">
-        <f>F9</f>
-        <v>16.5</v>
+        <v>150</v>
       </c>
       <c r="L9" s="6">
-        <f>K9</f>
-        <v>16.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -16732,7 +16730,7 @@
         <v>80</v>
       </c>
       <c r="K11" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L11" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
Fixing issue with construction properties DB
The Hochschulquartier case study includes a building from 1291. The
current archetype database has a start year of 1300, so the building in
question will create an error. The oldest start year was therefore
arbitrarily changed to 1000.
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_CH.xlsx
+++ b/cea/databases/archetypes/construction_properties_CH.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinmo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/C/Users/User/Documents/GitHub/CEAforArcGIS/cea/databases/archetypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23940" windowHeight="22020" tabRatio="785"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22060" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4072" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4000" uniqueCount="73">
   <si>
     <t>Code</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>2021</t>
-  </si>
-  <si>
-    <t>1300</t>
   </si>
   <si>
     <t>year_start</t>
@@ -1141,11 +1138,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E184" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1:J1048576"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1164,31 +1161,31 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>50</v>
@@ -1213,14 +1210,14 @@
       <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>63</v>
+      <c r="B2" s="7">
+        <v>1000</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="3">
         <v>0.82</v>
@@ -1268,7 +1265,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="3">
         <v>0.82</v>
@@ -1316,7 +1313,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" s="3">
         <v>0.82</v>
@@ -1364,7 +1361,7 @@
         <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" s="3">
         <v>0.82</v>
@@ -1412,7 +1409,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="3">
         <v>0.82</v>
@@ -1459,7 +1456,7 @@
         <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="3">
         <v>0.82</v>
@@ -1499,14 +1496,14 @@
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>63</v>
+      <c r="B8" s="7">
+        <v>1000</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="3">
         <v>0.82</v>
@@ -1553,7 +1550,7 @@
         <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" s="3">
         <v>0.82</v>
@@ -1600,7 +1597,7 @@
         <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="3">
         <v>0.82</v>
@@ -1647,7 +1644,7 @@
         <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="3">
         <v>0.82</v>
@@ -1694,7 +1691,7 @@
         <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" s="3">
         <v>0.82</v>
@@ -1741,7 +1738,7 @@
         <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="3">
         <v>0.82</v>
@@ -1781,14 +1778,14 @@
       <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>63</v>
+      <c r="B14" s="7">
+        <v>1000</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="3">
         <v>0.85</v>
@@ -1835,7 +1832,7 @@
         <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="3">
         <v>0.85</v>
@@ -1882,7 +1879,7 @@
         <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E16" s="3">
         <v>0.85</v>
@@ -1929,7 +1926,7 @@
         <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="3">
         <v>0.85</v>
@@ -1976,7 +1973,7 @@
         <v>59</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18" s="3">
         <v>0.85</v>
@@ -2023,7 +2020,7 @@
         <v>60</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" s="3">
         <v>0.85</v>
@@ -2063,14 +2060,14 @@
       <c r="A20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>63</v>
+      <c r="B20" s="7">
+        <v>1000</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="3">
         <v>0.85</v>
@@ -2117,7 +2114,7 @@
         <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="3">
         <v>0.85</v>
@@ -2164,7 +2161,7 @@
         <v>57</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E22" s="3">
         <v>0.85</v>
@@ -2211,7 +2208,7 @@
         <v>58</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E23" s="3">
         <v>0.85</v>
@@ -2258,7 +2255,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E24" s="3">
         <v>0.85</v>
@@ -2305,7 +2302,7 @@
         <v>60</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25" s="3">
         <v>0.85</v>
@@ -2345,14 +2342,14 @@
       <c r="A26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>63</v>
+      <c r="B26" s="7">
+        <v>1000</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E26" s="3">
         <v>0.9</v>
@@ -2399,7 +2396,7 @@
         <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E27" s="3">
         <v>0.9</v>
@@ -2446,7 +2443,7 @@
         <v>57</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E28" s="3">
         <v>0.9</v>
@@ -2493,7 +2490,7 @@
         <v>58</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E29" s="3">
         <v>0.9</v>
@@ -2540,7 +2537,7 @@
         <v>59</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E30" s="3">
         <v>0.9</v>
@@ -2587,7 +2584,7 @@
         <v>60</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E31" s="3">
         <v>0.9</v>
@@ -2627,14 +2624,14 @@
       <c r="A32" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>63</v>
+      <c r="B32" s="7">
+        <v>1000</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E32" s="3">
         <v>0.9</v>
@@ -2681,7 +2678,7 @@
         <v>56</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E33" s="3">
         <v>0.9</v>
@@ -2728,7 +2725,7 @@
         <v>57</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E34" s="3">
         <v>0.9</v>
@@ -2775,7 +2772,7 @@
         <v>58</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E35" s="3">
         <v>0.9</v>
@@ -2822,7 +2819,7 @@
         <v>59</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E36" s="3">
         <v>0.9</v>
@@ -2869,7 +2866,7 @@
         <v>60</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E37" s="3">
         <v>0.9</v>
@@ -2909,14 +2906,14 @@
       <c r="A38" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>63</v>
+      <c r="B38" s="7">
+        <v>1000</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E38" s="3">
         <v>0.9</v>
@@ -2963,7 +2960,7 @@
         <v>56</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E39" s="3">
         <v>0.9</v>
@@ -3010,7 +3007,7 @@
         <v>57</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E40" s="3">
         <v>0.9</v>
@@ -3057,7 +3054,7 @@
         <v>58</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E41" s="3">
         <v>0.9</v>
@@ -3104,7 +3101,7 @@
         <v>59</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E42" s="3">
         <v>0.9</v>
@@ -3151,7 +3148,7 @@
         <v>60</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E43" s="3">
         <v>0.9</v>
@@ -3191,14 +3188,14 @@
       <c r="A44" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>63</v>
+      <c r="B44" s="7">
+        <v>1000</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E44" s="3">
         <v>0.9</v>
@@ -3245,7 +3242,7 @@
         <v>56</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E45" s="3">
         <v>0.9</v>
@@ -3292,7 +3289,7 @@
         <v>57</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E46" s="3">
         <v>0.9</v>
@@ -3339,7 +3336,7 @@
         <v>58</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E47" s="3">
         <v>0.9</v>
@@ -3386,7 +3383,7 @@
         <v>59</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E48" s="3">
         <v>0.9</v>
@@ -3433,7 +3430,7 @@
         <v>60</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E49" s="3">
         <v>0.9</v>
@@ -3473,14 +3470,14 @@
       <c r="A50" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>63</v>
+      <c r="B50" s="7">
+        <v>1000</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E50" s="3">
         <v>0.9</v>
@@ -3527,7 +3524,7 @@
         <v>56</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E51" s="3">
         <v>0.9</v>
@@ -3574,7 +3571,7 @@
         <v>57</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E52" s="3">
         <v>0.9</v>
@@ -3621,7 +3618,7 @@
         <v>58</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E53" s="3">
         <v>0.9</v>
@@ -3668,7 +3665,7 @@
         <v>59</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E54" s="3">
         <v>0.9</v>
@@ -3715,7 +3712,7 @@
         <v>60</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E55" s="3">
         <v>0.9</v>
@@ -3755,14 +3752,14 @@
       <c r="A56" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>63</v>
+      <c r="B56" s="7">
+        <v>1000</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E56" s="3">
         <v>0.9</v>
@@ -3809,7 +3806,7 @@
         <v>56</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E57" s="3">
         <v>0.9</v>
@@ -3856,7 +3853,7 @@
         <v>57</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E58" s="3">
         <v>0.9</v>
@@ -3903,7 +3900,7 @@
         <v>58</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E59" s="3">
         <v>0.9</v>
@@ -3950,7 +3947,7 @@
         <v>59</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E60" s="3">
         <v>0.9</v>
@@ -3997,7 +3994,7 @@
         <v>60</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E61" s="3">
         <v>0.9</v>
@@ -4037,14 +4034,14 @@
       <c r="A62" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>63</v>
+      <c r="B62" s="7">
+        <v>1000</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E62" s="3">
         <v>0.9</v>
@@ -4091,7 +4088,7 @@
         <v>56</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E63" s="3">
         <v>0.9</v>
@@ -4138,7 +4135,7 @@
         <v>57</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E64" s="3">
         <v>0.9</v>
@@ -4185,7 +4182,7 @@
         <v>58</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E65" s="3">
         <v>0.9</v>
@@ -4232,7 +4229,7 @@
         <v>59</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E66" s="3">
         <v>0.9</v>
@@ -4279,7 +4276,7 @@
         <v>60</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E67" s="3">
         <v>0.9</v>
@@ -4319,14 +4316,14 @@
       <c r="A68" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>63</v>
+      <c r="B68" s="7">
+        <v>1000</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E68" s="3">
         <v>0.9</v>
@@ -4373,7 +4370,7 @@
         <v>56</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E69" s="3">
         <v>0.9</v>
@@ -4420,7 +4417,7 @@
         <v>57</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E70" s="3">
         <v>0.9</v>
@@ -4467,7 +4464,7 @@
         <v>58</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E71" s="3">
         <v>0.9</v>
@@ -4514,7 +4511,7 @@
         <v>59</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E72" s="3">
         <v>0.9</v>
@@ -4561,7 +4558,7 @@
         <v>60</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E73" s="3">
         <v>0.9</v>
@@ -4601,14 +4598,14 @@
       <c r="A74" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B74" s="7" t="s">
-        <v>63</v>
+      <c r="B74" s="7">
+        <v>1000</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E74" s="3">
         <v>0.9</v>
@@ -4655,7 +4652,7 @@
         <v>56</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E75" s="3">
         <v>0.9</v>
@@ -4702,7 +4699,7 @@
         <v>57</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E76" s="3">
         <v>0.9</v>
@@ -4749,7 +4746,7 @@
         <v>58</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E77" s="3">
         <v>0.9</v>
@@ -4796,7 +4793,7 @@
         <v>59</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E78" s="3">
         <v>0.9</v>
@@ -4843,7 +4840,7 @@
         <v>60</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E79" s="3">
         <v>0.9</v>
@@ -4883,14 +4880,14 @@
       <c r="A80" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B80" s="7" t="s">
-        <v>63</v>
+      <c r="B80" s="7">
+        <v>1000</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E80" s="3">
         <v>0.9</v>
@@ -4937,7 +4934,7 @@
         <v>56</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E81" s="3">
         <v>0.9</v>
@@ -4984,7 +4981,7 @@
         <v>57</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E82" s="3">
         <v>0.9</v>
@@ -5031,7 +5028,7 @@
         <v>58</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E83" s="3">
         <v>0.9</v>
@@ -5078,7 +5075,7 @@
         <v>59</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E84" s="3">
         <v>0.9</v>
@@ -5125,7 +5122,7 @@
         <v>60</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E85" s="3">
         <v>0.9</v>
@@ -5165,14 +5162,14 @@
       <c r="A86" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B86" s="7" t="s">
-        <v>63</v>
+      <c r="B86" s="7">
+        <v>1000</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E86" s="3">
         <v>0.9</v>
@@ -5219,7 +5216,7 @@
         <v>56</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E87" s="3">
         <v>0.9</v>
@@ -5266,7 +5263,7 @@
         <v>57</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E88" s="3">
         <v>0.9</v>
@@ -5313,7 +5310,7 @@
         <v>58</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E89" s="3">
         <v>0.9</v>
@@ -5360,7 +5357,7 @@
         <v>59</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E90" s="3">
         <v>0.9</v>
@@ -5407,7 +5404,7 @@
         <v>60</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E91" s="3">
         <v>0.9</v>
@@ -5447,14 +5444,14 @@
       <c r="A92" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B92" s="7" t="s">
-        <v>63</v>
+      <c r="B92" s="7">
+        <v>1000</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E92" s="3">
         <v>0.9</v>
@@ -5501,7 +5498,7 @@
         <v>56</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E93" s="3">
         <v>0.9</v>
@@ -5548,7 +5545,7 @@
         <v>57</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E94" s="3">
         <v>0.9</v>
@@ -5595,7 +5592,7 @@
         <v>58</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E95" s="3">
         <v>0.9</v>
@@ -5642,7 +5639,7 @@
         <v>59</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E96" s="3">
         <v>0.9</v>
@@ -5689,7 +5686,7 @@
         <v>60</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E97" s="3">
         <v>0.9</v>
@@ -5729,14 +5726,14 @@
       <c r="A98" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B98" s="7" t="s">
-        <v>63</v>
+      <c r="B98" s="7">
+        <v>1000</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E98" s="3">
         <v>0.9</v>
@@ -5783,7 +5780,7 @@
         <v>56</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E99" s="3">
         <v>0.9</v>
@@ -5830,7 +5827,7 @@
         <v>57</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E100" s="3">
         <v>0.9</v>
@@ -5877,7 +5874,7 @@
         <v>58</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E101" s="3">
         <v>0.9</v>
@@ -5924,7 +5921,7 @@
         <v>59</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E102" s="3">
         <v>0.9</v>
@@ -5971,7 +5968,7 @@
         <v>60</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E103" s="3">
         <v>0.9</v>
@@ -6011,14 +6008,14 @@
       <c r="A104" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B104" s="7" t="s">
-        <v>63</v>
+      <c r="B104" s="7">
+        <v>1000</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E104" s="3">
         <v>0.9</v>
@@ -6065,7 +6062,7 @@
         <v>56</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E105" s="3">
         <v>0.9</v>
@@ -6112,7 +6109,7 @@
         <v>57</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E106" s="3">
         <v>0.9</v>
@@ -6159,7 +6156,7 @@
         <v>58</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E107" s="3">
         <v>0.9</v>
@@ -6206,7 +6203,7 @@
         <v>59</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E108" s="3">
         <v>0.9</v>
@@ -6253,7 +6250,7 @@
         <v>60</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E109" s="3">
         <v>0.9</v>
@@ -6293,14 +6290,14 @@
       <c r="A110" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B110" s="7" t="s">
-        <v>63</v>
+      <c r="B110" s="7">
+        <v>1000</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E110" s="3">
         <v>0.9</v>
@@ -6347,7 +6344,7 @@
         <v>56</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E111" s="3">
         <v>0.9</v>
@@ -6394,7 +6391,7 @@
         <v>57</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E112" s="3">
         <v>0.9</v>
@@ -6441,7 +6438,7 @@
         <v>58</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E113" s="3">
         <v>0.9</v>
@@ -6488,7 +6485,7 @@
         <v>59</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E114" s="3">
         <v>0.9</v>
@@ -6535,7 +6532,7 @@
         <v>60</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E115" s="3">
         <v>0.9</v>
@@ -6575,14 +6572,14 @@
       <c r="A116" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B116" s="7" t="s">
-        <v>63</v>
+      <c r="B116" s="7">
+        <v>1000</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E116" s="3">
         <v>0.9</v>
@@ -6629,7 +6626,7 @@
         <v>56</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E117" s="3">
         <v>0.9</v>
@@ -6676,7 +6673,7 @@
         <v>57</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E118" s="3">
         <v>0.9</v>
@@ -6723,7 +6720,7 @@
         <v>58</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E119" s="3">
         <v>0.9</v>
@@ -6770,7 +6767,7 @@
         <v>59</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E120" s="3">
         <v>0.9</v>
@@ -6817,7 +6814,7 @@
         <v>60</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E121" s="3">
         <v>0.9</v>
@@ -6857,14 +6854,14 @@
       <c r="A122" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B122" s="7" t="s">
-        <v>63</v>
+      <c r="B122" s="7">
+        <v>1000</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E122" s="3">
         <v>0.9</v>
@@ -6911,7 +6908,7 @@
         <v>56</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E123" s="3">
         <v>0.9</v>
@@ -6958,7 +6955,7 @@
         <v>57</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E124" s="3">
         <v>0.9</v>
@@ -7005,7 +7002,7 @@
         <v>58</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E125" s="3">
         <v>0.9</v>
@@ -7052,7 +7049,7 @@
         <v>59</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E126" s="3">
         <v>0.9</v>
@@ -7099,7 +7096,7 @@
         <v>60</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E127" s="3">
         <v>0.9</v>
@@ -7139,14 +7136,14 @@
       <c r="A128" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B128" s="7" t="s">
-        <v>63</v>
+      <c r="B128" s="7">
+        <v>1000</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E128" s="3">
         <v>0.9</v>
@@ -7193,7 +7190,7 @@
         <v>56</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E129" s="3">
         <v>0.9</v>
@@ -7240,7 +7237,7 @@
         <v>57</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E130" s="3">
         <v>0.9</v>
@@ -7287,7 +7284,7 @@
         <v>58</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E131" s="3">
         <v>0.9</v>
@@ -7334,7 +7331,7 @@
         <v>59</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E132" s="3">
         <v>0.9</v>
@@ -7381,7 +7378,7 @@
         <v>60</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E133" s="3">
         <v>0.9</v>
@@ -7421,14 +7418,14 @@
       <c r="A134" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B134" s="7" t="s">
-        <v>63</v>
+      <c r="B134" s="7">
+        <v>1000</v>
       </c>
       <c r="C134" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E134" s="3">
         <v>0.9</v>
@@ -7475,7 +7472,7 @@
         <v>56</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E135" s="3">
         <v>0.9</v>
@@ -7522,7 +7519,7 @@
         <v>57</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E136" s="3">
         <v>0.9</v>
@@ -7569,7 +7566,7 @@
         <v>58</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E137" s="3">
         <v>0.9</v>
@@ -7616,7 +7613,7 @@
         <v>59</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E138" s="3">
         <v>0.9</v>
@@ -7663,7 +7660,7 @@
         <v>60</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E139" s="3">
         <v>0.9</v>
@@ -7703,14 +7700,14 @@
       <c r="A140" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B140" s="7" t="s">
-        <v>63</v>
+      <c r="B140" s="7">
+        <v>1000</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E140" s="3">
         <v>0.9</v>
@@ -7757,7 +7754,7 @@
         <v>56</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E141" s="3">
         <v>0.9</v>
@@ -7804,7 +7801,7 @@
         <v>57</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E142" s="3">
         <v>0.9</v>
@@ -7851,7 +7848,7 @@
         <v>58</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E143" s="3">
         <v>0.9</v>
@@ -7898,7 +7895,7 @@
         <v>59</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E144" s="3">
         <v>0.9</v>
@@ -7945,7 +7942,7 @@
         <v>60</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E145" s="3">
         <v>0.9</v>
@@ -7985,14 +7982,14 @@
       <c r="A146" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B146" s="7" t="s">
-        <v>63</v>
+      <c r="B146" s="7">
+        <v>1000</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E146" s="3">
         <v>1</v>
@@ -8039,7 +8036,7 @@
         <v>56</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E147" s="3">
         <v>1</v>
@@ -8086,7 +8083,7 @@
         <v>57</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E148" s="3">
         <v>1</v>
@@ -8133,7 +8130,7 @@
         <v>58</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E149" s="3">
         <v>1</v>
@@ -8180,7 +8177,7 @@
         <v>59</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E150" s="3">
         <v>1</v>
@@ -8227,7 +8224,7 @@
         <v>60</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E151" s="3">
         <v>1</v>
@@ -8267,14 +8264,14 @@
       <c r="A152" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B152" s="7" t="s">
-        <v>63</v>
+      <c r="B152" s="7">
+        <v>1000</v>
       </c>
       <c r="C152" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E152" s="3">
         <v>1</v>
@@ -8321,7 +8318,7 @@
         <v>56</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E153" s="3">
         <v>1</v>
@@ -8368,7 +8365,7 @@
         <v>57</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E154" s="3">
         <v>1</v>
@@ -8415,7 +8412,7 @@
         <v>58</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E155" s="3">
         <v>1</v>
@@ -8462,7 +8459,7 @@
         <v>59</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E156" s="3">
         <v>1</v>
@@ -8509,7 +8506,7 @@
         <v>60</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E157" s="3">
         <v>1</v>
@@ -8549,14 +8546,14 @@
       <c r="A158" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B158" s="7" t="s">
-        <v>63</v>
+      <c r="B158" s="7">
+        <v>1000</v>
       </c>
       <c r="C158" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E158" s="3">
         <v>0</v>
@@ -8603,7 +8600,7 @@
         <v>56</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E159" s="3">
         <v>0</v>
@@ -8650,7 +8647,7 @@
         <v>57</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E160" s="3">
         <v>0</v>
@@ -8697,7 +8694,7 @@
         <v>58</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E161" s="3">
         <v>0</v>
@@ -8744,7 +8741,7 @@
         <v>59</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E162" s="3">
         <v>0</v>
@@ -8791,7 +8788,7 @@
         <v>60</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E163" s="3">
         <v>0</v>
@@ -8831,14 +8828,14 @@
       <c r="A164" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B164" s="7" t="s">
-        <v>63</v>
+      <c r="B164" s="7">
+        <v>1000</v>
       </c>
       <c r="C164" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E164" s="3">
         <v>0</v>
@@ -8885,7 +8882,7 @@
         <v>56</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E165" s="3">
         <v>0</v>
@@ -8932,7 +8929,7 @@
         <v>57</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E166" s="3">
         <v>0</v>
@@ -8979,7 +8976,7 @@
         <v>58</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E167" s="3">
         <v>0</v>
@@ -9026,7 +9023,7 @@
         <v>59</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E168" s="3">
         <v>0</v>
@@ -9073,7 +9070,7 @@
         <v>60</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E169" s="3">
         <v>0</v>
@@ -9113,14 +9110,14 @@
       <c r="A170" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B170" s="7" t="s">
-        <v>63</v>
+      <c r="B170" s="7">
+        <v>1000</v>
       </c>
       <c r="C170" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E170" s="3">
         <v>0</v>
@@ -9167,7 +9164,7 @@
         <v>56</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E171" s="3">
         <v>0</v>
@@ -9214,7 +9211,7 @@
         <v>57</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E172" s="3">
         <v>0</v>
@@ -9261,7 +9258,7 @@
         <v>58</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E173" s="3">
         <v>0</v>
@@ -9308,7 +9305,7 @@
         <v>59</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E174" s="3">
         <v>0</v>
@@ -9355,7 +9352,7 @@
         <v>60</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E175" s="3">
         <v>0</v>
@@ -9395,14 +9392,14 @@
       <c r="A176" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B176" s="7" t="s">
-        <v>63</v>
+      <c r="B176" s="7">
+        <v>1000</v>
       </c>
       <c r="C176" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E176" s="3">
         <v>0</v>
@@ -9449,7 +9446,7 @@
         <v>56</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E177" s="3">
         <v>0</v>
@@ -9496,7 +9493,7 @@
         <v>57</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E178" s="3">
         <v>0</v>
@@ -9543,7 +9540,7 @@
         <v>58</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E179" s="3">
         <v>0</v>
@@ -9590,7 +9587,7 @@
         <v>59</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E180" s="3">
         <v>0</v>
@@ -9637,7 +9634,7 @@
         <v>60</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E181" s="3">
         <v>0</v>
@@ -9677,14 +9674,14 @@
       <c r="A182" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B182" s="7" t="s">
-        <v>63</v>
+      <c r="B182" s="7">
+        <v>1000</v>
       </c>
       <c r="C182" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E182" s="3">
         <f>E86</f>
@@ -9737,7 +9734,7 @@
         <v>56</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E183" s="3">
         <f t="shared" ref="E183:E193" si="1">E87</f>
@@ -9790,7 +9787,7 @@
         <v>57</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E184" s="3">
         <f t="shared" si="1"/>
@@ -9843,7 +9840,7 @@
         <v>58</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E185" s="3">
         <f t="shared" si="1"/>
@@ -9896,7 +9893,7 @@
         <v>59</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E186" s="3">
         <f t="shared" si="1"/>
@@ -9949,7 +9946,7 @@
         <v>60</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E187" s="3">
         <f t="shared" si="1"/>
@@ -9995,14 +9992,14 @@
       <c r="A188" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B188" s="7" t="s">
-        <v>63</v>
+      <c r="B188" s="7">
+        <v>1000</v>
       </c>
       <c r="C188" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E188" s="3">
         <f t="shared" si="1"/>
@@ -10055,7 +10052,7 @@
         <v>56</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E189" s="3">
         <f t="shared" si="1"/>
@@ -10108,7 +10105,7 @@
         <v>57</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E190" s="3">
         <f t="shared" si="1"/>
@@ -10161,7 +10158,7 @@
         <v>58</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E191" s="3">
         <f t="shared" si="1"/>
@@ -10214,7 +10211,7 @@
         <v>59</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E192" s="3">
         <f t="shared" si="1"/>
@@ -10267,7 +10264,7 @@
         <v>60</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E193" s="3">
         <f t="shared" si="1"/>
@@ -10313,14 +10310,14 @@
       <c r="A194" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B194" s="7" t="s">
-        <v>63</v>
+      <c r="B194" s="7">
+        <v>1000</v>
       </c>
       <c r="C194" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E194" s="3">
         <f t="shared" ref="E194:E205" si="4">E182</f>
@@ -10369,7 +10366,7 @@
         <v>56</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E195" s="3">
         <f t="shared" si="4"/>
@@ -10418,7 +10415,7 @@
         <v>57</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E196" s="3">
         <f t="shared" si="4"/>
@@ -10467,7 +10464,7 @@
         <v>58</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E197" s="3">
         <f t="shared" si="4"/>
@@ -10516,7 +10513,7 @@
         <v>59</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E198" s="3">
         <f t="shared" si="4"/>
@@ -10565,7 +10562,7 @@
         <v>60</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E199" s="3">
         <f t="shared" si="4"/>
@@ -10607,14 +10604,14 @@
       <c r="A200" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B200" s="7" t="s">
-        <v>63</v>
+      <c r="B200" s="7">
+        <v>1000</v>
       </c>
       <c r="C200" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E200" s="3">
         <f t="shared" si="4"/>
@@ -10663,7 +10660,7 @@
         <v>56</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E201" s="3">
         <f t="shared" si="4"/>
@@ -10712,7 +10709,7 @@
         <v>57</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E202" s="3">
         <f t="shared" si="4"/>
@@ -10761,7 +10758,7 @@
         <v>58</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E203" s="3">
         <f t="shared" si="4"/>
@@ -10810,7 +10807,7 @@
         <v>59</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E204" s="3">
         <f t="shared" si="4"/>
@@ -10859,7 +10856,7 @@
         <v>60</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E205" s="3">
         <f t="shared" si="4"/>
@@ -10901,14 +10898,14 @@
       <c r="A206" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B206" s="7" t="s">
-        <v>63</v>
+      <c r="B206" s="7">
+        <v>1000</v>
       </c>
       <c r="C206" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E206" s="3">
         <v>0.9</v>
@@ -10955,7 +10952,7 @@
         <v>56</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E207" s="3">
         <v>0.9</v>
@@ -11002,7 +10999,7 @@
         <v>57</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E208" s="3">
         <v>0.9</v>
@@ -11049,7 +11046,7 @@
         <v>58</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E209" s="3">
         <v>0.9</v>
@@ -11096,7 +11093,7 @@
         <v>59</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E210" s="3">
         <v>0.9</v>
@@ -11143,7 +11140,7 @@
         <v>60</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E211" s="3">
         <v>0.9</v>
@@ -11183,14 +11180,14 @@
       <c r="A212" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B212" s="7" t="s">
-        <v>63</v>
+      <c r="B212" s="7">
+        <v>1000</v>
       </c>
       <c r="C212" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E212" s="3">
         <v>0.9</v>
@@ -11237,7 +11234,7 @@
         <v>56</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E213" s="3">
         <v>0.9</v>
@@ -11284,7 +11281,7 @@
         <v>57</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E214" s="3">
         <v>0.9</v>
@@ -11331,7 +11328,7 @@
         <v>58</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E215" s="3">
         <v>0.9</v>
@@ -11378,7 +11375,7 @@
         <v>59</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E216" s="3">
         <v>0.9</v>
@@ -11425,7 +11422,7 @@
         <v>60</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E217" s="3">
         <v>0.9</v>
@@ -11465,7 +11462,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:C7 B8:C13 B14:C25 B26:C37 B38:C49 B50:C61 B62:C121 B122:C181 B182:C217" numberStoredAsText="1"/>
+    <ignoredError sqref="B3:C7 B9:C13 B15:C19 B27:C31 B39:C43 B51:C55 B63:C67 B123:C127 B183:C187 C2 C8 C14 B21:C25 C20 C26 B33:C37 C32 C38 B45:C49 C44 C50 B57:C61 C56 C62 B69:C73 C68 B75:C79 C74 B81:C85 C80 B87:C91 C86 B93:C97 C92 B99:C103 C98 B105:C109 C104 B111:C115 C110 B117:C121 C116 C122 B129:C133 C128 B135:C139 C134 B141:C145 C140 B147:C151 C146 B153:C157 C152 B159:C163 C158 B165:C169 C164 B171:C175 C170 B177:C181 C176 C182 B189:C193 C188 B195:C199 C194 B201:C205 C200 B207:C211 C206 B213:C217 C212" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -11478,13 +11475,13 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E144" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H158" sqref="H158"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" style="14" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.1640625" style="4"/>
@@ -11496,16 +11493,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>2</v>
@@ -11527,14 +11524,14 @@
       <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>63</v>
+      <c r="B2" s="7">
+        <v>1000</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>8</v>
@@ -11563,7 +11560,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
@@ -11592,7 +11589,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>8</v>
@@ -11621,7 +11618,7 @@
         <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>8</v>
@@ -11650,7 +11647,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>11</v>
@@ -11679,7 +11676,7 @@
         <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
@@ -11701,14 +11698,14 @@
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>63</v>
+      <c r="B8" s="7">
+        <v>1000</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>8</v>
@@ -11737,7 +11734,7 @@
         <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>8</v>
@@ -11766,7 +11763,7 @@
         <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>8</v>
@@ -11795,7 +11792,7 @@
         <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>8</v>
@@ -11824,7 +11821,7 @@
         <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>11</v>
@@ -11853,7 +11850,7 @@
         <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>11</v>
@@ -11875,14 +11872,14 @@
       <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>63</v>
+      <c r="B14" s="7">
+        <v>1000</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>8</v>
@@ -11911,7 +11908,7 @@
         <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>8</v>
@@ -11940,7 +11937,7 @@
         <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>8</v>
@@ -11969,7 +11966,7 @@
         <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>8</v>
@@ -11998,7 +11995,7 @@
         <v>59</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>11</v>
@@ -12027,7 +12024,7 @@
         <v>60</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>11</v>
@@ -12049,14 +12046,14 @@
       <c r="A20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>63</v>
+      <c r="B20" s="7">
+        <v>1000</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>8</v>
@@ -12085,7 +12082,7 @@
         <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>8</v>
@@ -12114,7 +12111,7 @@
         <v>57</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>8</v>
@@ -12143,7 +12140,7 @@
         <v>58</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>8</v>
@@ -12172,7 +12169,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>11</v>
@@ -12201,7 +12198,7 @@
         <v>60</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>11</v>
@@ -12223,14 +12220,14 @@
       <c r="A26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>63</v>
+      <c r="B26" s="7">
+        <v>1000</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -12259,7 +12256,7 @@
         <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -12288,7 +12285,7 @@
         <v>57</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -12317,7 +12314,7 @@
         <v>58</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -12346,7 +12343,7 @@
         <v>59</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>10</v>
@@ -12375,7 +12372,7 @@
         <v>60</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>10</v>
@@ -12397,14 +12394,14 @@
       <c r="A32" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>63</v>
+      <c r="B32" s="7">
+        <v>1000</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -12433,7 +12430,7 @@
         <v>56</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -12462,7 +12459,7 @@
         <v>57</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -12491,7 +12488,7 @@
         <v>58</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -12520,7 +12517,7 @@
         <v>59</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>10</v>
@@ -12549,7 +12546,7 @@
         <v>60</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>10</v>
@@ -12571,14 +12568,14 @@
       <c r="A38" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>63</v>
+      <c r="B38" s="7">
+        <v>1000</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -12607,7 +12604,7 @@
         <v>56</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -12636,7 +12633,7 @@
         <v>57</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -12665,7 +12662,7 @@
         <v>58</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -12694,7 +12691,7 @@
         <v>59</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>10</v>
@@ -12723,7 +12720,7 @@
         <v>60</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>7</v>
@@ -12745,14 +12742,14 @@
       <c r="A44" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>63</v>
+      <c r="B44" s="7">
+        <v>1000</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -12781,7 +12778,7 @@
         <v>56</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -12810,7 +12807,7 @@
         <v>57</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -12839,7 +12836,7 @@
         <v>58</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -12868,7 +12865,7 @@
         <v>59</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>10</v>
@@ -12897,7 +12894,7 @@
         <v>60</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>7</v>
@@ -12919,14 +12916,14 @@
       <c r="A50" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>63</v>
+      <c r="B50" s="7">
+        <v>1000</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -12955,7 +12952,7 @@
         <v>56</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -12984,7 +12981,7 @@
         <v>57</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -13013,7 +13010,7 @@
         <v>58</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -13042,7 +13039,7 @@
         <v>59</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>7</v>
@@ -13071,7 +13068,7 @@
         <v>60</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>7</v>
@@ -13093,14 +13090,14 @@
       <c r="A56" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>63</v>
+      <c r="B56" s="7">
+        <v>1000</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>7</v>
@@ -13129,7 +13126,7 @@
         <v>56</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>7</v>
@@ -13158,7 +13155,7 @@
         <v>57</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>7</v>
@@ -13187,7 +13184,7 @@
         <v>58</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>7</v>
@@ -13216,7 +13213,7 @@
         <v>59</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>7</v>
@@ -13245,7 +13242,7 @@
         <v>60</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>7</v>
@@ -13267,14 +13264,14 @@
       <c r="A62" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>63</v>
+      <c r="B62" s="7">
+        <v>1000</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -13303,7 +13300,7 @@
         <v>56</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -13332,7 +13329,7 @@
         <v>57</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -13361,7 +13358,7 @@
         <v>58</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -13390,7 +13387,7 @@
         <v>59</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -13419,7 +13416,7 @@
         <v>60</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>7</v>
@@ -13441,14 +13438,14 @@
       <c r="A68" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>63</v>
+      <c r="B68" s="7">
+        <v>1000</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>7</v>
@@ -13477,7 +13474,7 @@
         <v>56</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>7</v>
@@ -13506,7 +13503,7 @@
         <v>57</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>7</v>
@@ -13535,7 +13532,7 @@
         <v>58</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>7</v>
@@ -13564,7 +13561,7 @@
         <v>59</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>7</v>
@@ -13593,7 +13590,7 @@
         <v>60</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>7</v>
@@ -13615,14 +13612,14 @@
       <c r="A74" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B74" s="7" t="s">
-        <v>63</v>
+      <c r="B74" s="7">
+        <v>1000</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -13651,7 +13648,7 @@
         <v>56</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -13680,7 +13677,7 @@
         <v>57</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>8</v>
@@ -13709,7 +13706,7 @@
         <v>58</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>8</v>
@@ -13738,7 +13735,7 @@
         <v>59</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
@@ -13767,7 +13764,7 @@
         <v>60</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>8</v>
@@ -13789,14 +13786,14 @@
       <c r="A80" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B80" s="7" t="s">
-        <v>63</v>
+      <c r="B80" s="7">
+        <v>1000</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>7</v>
@@ -13825,7 +13822,7 @@
         <v>56</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>7</v>
@@ -13854,7 +13851,7 @@
         <v>57</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>7</v>
@@ -13883,7 +13880,7 @@
         <v>58</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>7</v>
@@ -13912,7 +13909,7 @@
         <v>59</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>8</v>
@@ -13941,7 +13938,7 @@
         <v>60</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -13963,14 +13960,14 @@
       <c r="A86" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B86" s="7" t="s">
-        <v>63</v>
+      <c r="B86" s="7">
+        <v>1000</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -13999,7 +13996,7 @@
         <v>56</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -14028,7 +14025,7 @@
         <v>57</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -14057,7 +14054,7 @@
         <v>58</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -14086,7 +14083,7 @@
         <v>59</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>7</v>
@@ -14115,7 +14112,7 @@
         <v>60</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>7</v>
@@ -14137,14 +14134,14 @@
       <c r="A92" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B92" s="7" t="s">
-        <v>63</v>
+      <c r="B92" s="7">
+        <v>1000</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -14173,7 +14170,7 @@
         <v>56</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -14202,7 +14199,7 @@
         <v>57</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -14231,7 +14228,7 @@
         <v>58</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -14260,7 +14257,7 @@
         <v>59</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>7</v>
@@ -14289,7 +14286,7 @@
         <v>60</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>7</v>
@@ -14311,14 +14308,14 @@
       <c r="A98" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B98" s="7" t="s">
-        <v>63</v>
+      <c r="B98" s="7">
+        <v>1000</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -14347,7 +14344,7 @@
         <v>56</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -14376,7 +14373,7 @@
         <v>57</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -14405,7 +14402,7 @@
         <v>58</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -14434,7 +14431,7 @@
         <v>59</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>7</v>
@@ -14463,7 +14460,7 @@
         <v>60</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>7</v>
@@ -14485,14 +14482,14 @@
       <c r="A104" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B104" s="7" t="s">
-        <v>63</v>
+      <c r="B104" s="7">
+        <v>1000</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -14521,7 +14518,7 @@
         <v>56</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -14550,7 +14547,7 @@
         <v>57</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -14579,7 +14576,7 @@
         <v>58</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>7</v>
@@ -14608,7 +14605,7 @@
         <v>59</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>7</v>
@@ -14637,7 +14634,7 @@
         <v>60</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>7</v>
@@ -14659,14 +14656,14 @@
       <c r="A110" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B110" s="7" t="s">
-        <v>63</v>
+      <c r="B110" s="7">
+        <v>1000</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -14695,7 +14692,7 @@
         <v>56</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -14724,7 +14721,7 @@
         <v>57</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -14753,7 +14750,7 @@
         <v>58</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -14782,7 +14779,7 @@
         <v>59</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>7</v>
@@ -14811,7 +14808,7 @@
         <v>60</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>7</v>
@@ -14833,14 +14830,14 @@
       <c r="A116" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B116" s="7" t="s">
-        <v>63</v>
+      <c r="B116" s="7">
+        <v>1000</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -14869,7 +14866,7 @@
         <v>56</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -14898,7 +14895,7 @@
         <v>57</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -14927,7 +14924,7 @@
         <v>58</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>7</v>
@@ -14956,7 +14953,7 @@
         <v>59</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>7</v>
@@ -14985,7 +14982,7 @@
         <v>60</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>7</v>
@@ -15007,14 +15004,14 @@
       <c r="A122" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B122" s="7" t="s">
-        <v>63</v>
+      <c r="B122" s="7">
+        <v>1000</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -15043,7 +15040,7 @@
         <v>56</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -15072,7 +15069,7 @@
         <v>57</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>7</v>
@@ -15101,7 +15098,7 @@
         <v>58</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>7</v>
@@ -15130,7 +15127,7 @@
         <v>59</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>7</v>
@@ -15159,7 +15156,7 @@
         <v>60</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>7</v>
@@ -15181,14 +15178,14 @@
       <c r="A128" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B128" s="7" t="s">
-        <v>63</v>
+      <c r="B128" s="7">
+        <v>1000</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>7</v>
@@ -15217,7 +15214,7 @@
         <v>56</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>7</v>
@@ -15246,7 +15243,7 @@
         <v>57</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>7</v>
@@ -15275,7 +15272,7 @@
         <v>58</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>7</v>
@@ -15304,7 +15301,7 @@
         <v>59</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>7</v>
@@ -15333,7 +15330,7 @@
         <v>60</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>7</v>
@@ -15355,14 +15352,14 @@
       <c r="A134" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B134" s="7" t="s">
-        <v>63</v>
+      <c r="B134" s="7">
+        <v>1000</v>
       </c>
       <c r="C134" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -15391,7 +15388,7 @@
         <v>56</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -15420,7 +15417,7 @@
         <v>57</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -15449,7 +15446,7 @@
         <v>58</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -15478,7 +15475,7 @@
         <v>59</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>11</v>
@@ -15507,7 +15504,7 @@
         <v>60</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>11</v>
@@ -15529,14 +15526,14 @@
       <c r="A140" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B140" s="7" t="s">
-        <v>63</v>
+      <c r="B140" s="7">
+        <v>1000</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -15565,7 +15562,7 @@
         <v>56</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -15594,7 +15591,7 @@
         <v>57</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -15623,7 +15620,7 @@
         <v>58</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -15652,7 +15649,7 @@
         <v>59</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>11</v>
@@ -15681,7 +15678,7 @@
         <v>60</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>11</v>
@@ -15703,14 +15700,14 @@
       <c r="A146" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B146" s="7" t="s">
-        <v>63</v>
+      <c r="B146" s="7">
+        <v>1000</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>9</v>
@@ -15739,7 +15736,7 @@
         <v>56</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>9</v>
@@ -15768,7 +15765,7 @@
         <v>57</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>9</v>
@@ -15797,7 +15794,7 @@
         <v>58</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>9</v>
@@ -15826,7 +15823,7 @@
         <v>59</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>9</v>
@@ -15855,7 +15852,7 @@
         <v>60</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>9</v>
@@ -15877,14 +15874,14 @@
       <c r="A152" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B152" s="7" t="s">
-        <v>63</v>
+      <c r="B152" s="7">
+        <v>1000</v>
       </c>
       <c r="C152" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>9</v>
@@ -15913,7 +15910,7 @@
         <v>56</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>9</v>
@@ -15942,7 +15939,7 @@
         <v>57</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>9</v>
@@ -15971,7 +15968,7 @@
         <v>58</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>9</v>
@@ -16000,7 +15997,7 @@
         <v>59</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>9</v>
@@ -16029,7 +16026,7 @@
         <v>60</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>9</v>
@@ -16051,14 +16048,14 @@
       <c r="A158" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B158" s="7" t="s">
-        <v>63</v>
+      <c r="B158" s="7">
+        <v>1000</v>
       </c>
       <c r="C158" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>9</v>
@@ -16087,7 +16084,7 @@
         <v>56</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>9</v>
@@ -16116,7 +16113,7 @@
         <v>57</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>9</v>
@@ -16145,7 +16142,7 @@
         <v>58</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>9</v>
@@ -16174,7 +16171,7 @@
         <v>59</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>9</v>
@@ -16203,7 +16200,7 @@
         <v>60</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>9</v>
@@ -16225,14 +16222,14 @@
       <c r="A164" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B164" s="7" t="s">
-        <v>63</v>
+      <c r="B164" s="7">
+        <v>1000</v>
       </c>
       <c r="C164" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>9</v>
@@ -16261,7 +16258,7 @@
         <v>56</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>9</v>
@@ -16290,7 +16287,7 @@
         <v>57</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>9</v>
@@ -16319,7 +16316,7 @@
         <v>58</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>9</v>
@@ -16348,7 +16345,7 @@
         <v>59</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>9</v>
@@ -16377,7 +16374,7 @@
         <v>60</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>9</v>
@@ -16399,14 +16396,14 @@
       <c r="A170" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B170" s="7" t="s">
-        <v>63</v>
+      <c r="B170" s="7">
+        <v>1000</v>
       </c>
       <c r="C170" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>9</v>
@@ -16435,7 +16432,7 @@
         <v>56</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>9</v>
@@ -16464,7 +16461,7 @@
         <v>57</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>9</v>
@@ -16493,7 +16490,7 @@
         <v>58</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>9</v>
@@ -16522,7 +16519,7 @@
         <v>59</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>9</v>
@@ -16551,7 +16548,7 @@
         <v>60</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>9</v>
@@ -16573,14 +16570,14 @@
       <c r="A176" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B176" s="7" t="s">
-        <v>63</v>
+      <c r="B176" s="7">
+        <v>1000</v>
       </c>
       <c r="C176" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>9</v>
@@ -16609,7 +16606,7 @@
         <v>56</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>9</v>
@@ -16638,7 +16635,7 @@
         <v>57</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>9</v>
@@ -16667,7 +16664,7 @@
         <v>58</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>9</v>
@@ -16696,7 +16693,7 @@
         <v>59</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>9</v>
@@ -16725,7 +16722,7 @@
         <v>60</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>9</v>
@@ -16747,14 +16744,14 @@
       <c r="A182" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B182" s="7" t="s">
-        <v>63</v>
+      <c r="B182" s="7">
+        <v>1000</v>
       </c>
       <c r="C182" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E182" s="3" t="str">
         <f>E86</f>
@@ -16788,7 +16785,7 @@
         <v>56</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E183" s="3" t="str">
         <f t="shared" ref="E183:E193" si="0">E87</f>
@@ -16822,7 +16819,7 @@
         <v>57</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E184" s="3" t="str">
         <f t="shared" si="0"/>
@@ -16856,7 +16853,7 @@
         <v>58</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E185" s="3" t="str">
         <f t="shared" si="0"/>
@@ -16890,7 +16887,7 @@
         <v>59</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E186" s="3" t="str">
         <f t="shared" si="0"/>
@@ -16924,7 +16921,7 @@
         <v>60</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E187" s="3" t="str">
         <f t="shared" si="0"/>
@@ -16951,14 +16948,14 @@
       <c r="A188" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B188" s="7" t="s">
-        <v>63</v>
+      <c r="B188" s="7">
+        <v>1000</v>
       </c>
       <c r="C188" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E188" s="3" t="str">
         <f t="shared" si="0"/>
@@ -16992,7 +16989,7 @@
         <v>56</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E189" s="3" t="str">
         <f t="shared" si="0"/>
@@ -17026,7 +17023,7 @@
         <v>57</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E190" s="3" t="str">
         <f t="shared" si="0"/>
@@ -17060,7 +17057,7 @@
         <v>58</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E191" s="3" t="str">
         <f t="shared" si="0"/>
@@ -17094,7 +17091,7 @@
         <v>59</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E192" s="3" t="str">
         <f t="shared" si="0"/>
@@ -17128,7 +17125,7 @@
         <v>60</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E193" s="3" t="str">
         <f t="shared" si="0"/>
@@ -17155,14 +17152,14 @@
       <c r="A194" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B194" s="7" t="s">
-        <v>63</v>
+      <c r="B194" s="7">
+        <v>1000</v>
       </c>
       <c r="C194" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>8</v>
@@ -17193,7 +17190,7 @@
         <v>56</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>8</v>
@@ -17224,7 +17221,7 @@
         <v>57</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>8</v>
@@ -17255,7 +17252,7 @@
         <v>58</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>8</v>
@@ -17286,7 +17283,7 @@
         <v>59</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>7</v>
@@ -17317,7 +17314,7 @@
         <v>60</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>7</v>
@@ -17341,14 +17338,14 @@
       <c r="A200" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B200" s="7" t="s">
-        <v>63</v>
+      <c r="B200" s="7">
+        <v>1000</v>
       </c>
       <c r="C200" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>8</v>
@@ -17379,7 +17376,7 @@
         <v>56</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>8</v>
@@ -17410,7 +17407,7 @@
         <v>57</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>8</v>
@@ -17441,7 +17438,7 @@
         <v>58</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>7</v>
@@ -17472,7 +17469,7 @@
         <v>59</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>7</v>
@@ -17503,7 +17500,7 @@
         <v>60</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E205" s="3" t="s">
         <v>7</v>
@@ -17527,14 +17524,14 @@
       <c r="A206" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B206" s="7" t="s">
-        <v>63</v>
+      <c r="B206" s="7">
+        <v>1000</v>
       </c>
       <c r="C206" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>8</v>
@@ -17563,7 +17560,7 @@
         <v>56</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>8</v>
@@ -17592,7 +17589,7 @@
         <v>57</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>8</v>
@@ -17621,7 +17618,7 @@
         <v>58</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>8</v>
@@ -17650,7 +17647,7 @@
         <v>59</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>7</v>
@@ -17679,7 +17676,7 @@
         <v>60</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E211" s="3" t="s">
         <v>7</v>
@@ -17701,14 +17698,14 @@
       <c r="A212" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B212" s="7" t="s">
-        <v>63</v>
+      <c r="B212" s="7">
+        <v>1000</v>
       </c>
       <c r="C212" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>8</v>
@@ -17737,7 +17734,7 @@
         <v>56</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E213" s="3" t="s">
         <v>8</v>
@@ -17766,7 +17763,7 @@
         <v>57</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E214" s="3" t="s">
         <v>8</v>
@@ -17795,7 +17792,7 @@
         <v>58</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>7</v>
@@ -17824,7 +17821,7 @@
         <v>59</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E216" s="3" t="s">
         <v>7</v>
@@ -17853,7 +17850,7 @@
         <v>60</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E217" s="3" t="s">
         <v>7</v>
@@ -18288,7 +18285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>

</xml_diff>